<commit_message>
make dump_results() for reviewing results of many simul. runs, and run_multialg() for testing a suite of multialgorithmic models; create a verification test for run_multialg, testing/multialgorithmic/00007/00007-wc_lang.xlsx; make 2 multialg test cases in verification/cases/multialgorithmic, 00007-wc_lang.xlsx and 00030-wc_lang.xlsx
</commit_message>
<xml_diff>
--- a/tests/fixtures/verification/cases/multialgorithmic/00030/00030-wc_lang.xlsx
+++ b/tests/fixtures/verification/cases/multialgorithmic/00030/00030-wc_lang.xlsx
@@ -5,12 +5,13 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/fixtures/verification/cases/stochastic/00030/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/fixtures/verification/cases/multialgorithmic/00030/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-27760" yWindow="8400" windowWidth="21280" windowHeight="5440" firstSheet="9" activeTab="12"/>
-    <workbookView xWindow="-22100" yWindow="520" windowWidth="18700" windowHeight="7860" tabRatio="500" firstSheet="15" activeTab="16"/>
+    <workbookView xWindow="580" yWindow="8520" windowWidth="28840" windowHeight="5220" firstSheet="9" activeTab="11"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="35800" windowHeight="5380" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="1080" yWindow="13840" windowWidth="27360" windowHeight="5780" tabRatio="500" firstSheet="9" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -4229,7 +4230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="201">
   <si>
     <t>!!!ObjTables ObjTablesVersion='0.0.8' Date='2019-12-05 16:22:38'</t>
   </si>
@@ -4705,9 +4706,6 @@
     <t>cellular_compartment</t>
   </si>
   <si>
-    <t>fluid_compartment</t>
-  </si>
-  <si>
     <t>gram</t>
   </si>
   <si>
@@ -4816,13 +4814,25 @@
     <t>k2</t>
   </si>
   <si>
-    <t>test_case_00030</t>
-  </si>
-  <si>
     <t>(k1 * P[c] * (P[c] - one)) / 2</t>
   </si>
   <si>
     <t>one</t>
+  </si>
+  <si>
+    <t>test_case_00030_multialgorithmic</t>
+  </si>
+  <si>
+    <t>ode_submodel</t>
+  </si>
+  <si>
+    <t>ODE submodel</t>
+  </si>
+  <si>
+    <t>ordinary_differential_equations</t>
+  </si>
+  <si>
+    <t>abstract_compartment</t>
   </si>
 </sst>
 </file>
@@ -4832,7 +4842,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4870,6 +4880,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -4936,10 +4954,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4982,9 +5001,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="11" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -5017,12 +5033,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5030,8 +5040,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5338,6 +5355,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5626,7 +5644,10 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5821,7 +5842,10 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6010,11 +6034,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6047,13 +6074,13 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="30" t="s">
         <v>86</v>
       </c>
       <c r="J2" s="5"/>
@@ -6108,22 +6135,22 @@
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -6136,22 +6163,22 @@
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -6296,7 +6323,7 @@
     <mergeCell ref="G2:I2"/>
   </mergeCells>
   <dataValidations count="14">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A4:A13 C4:C5">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A4:A13 C5">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
@@ -6352,11 +6379,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6387,60 +6415,60 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="20" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -6450,21 +6478,21 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -6585,6 +6613,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6839,6 +6868,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7062,6 +7092,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7302,18 +7333,21 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="1"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="1"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="2">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="24" bestFit="1" customWidth="1"/>
     <col min="7" max="11" width="15.6640625" customWidth="1"/>
     <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
   </cols>
@@ -7324,9 +7358,9 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="22"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="21"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -7334,22 +7368,22 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="22" t="s">
         <v>66</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -7370,41 +7404,41 @@
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="20">
+      <c r="D3" s="19">
         <v>1</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="19">
         <v>0</v>
       </c>
-      <c r="F3" s="24" t="s">
-        <v>173</v>
+      <c r="F3" s="23" t="s">
+        <v>172</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
-        <v>166</v>
-      </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="20">
+      <c r="A4" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="19">
         <v>1E-3</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="19">
         <v>0</v>
       </c>
-      <c r="F4" s="24" t="s">
-        <v>193</v>
+      <c r="F4" s="23" t="s">
+        <v>192</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -7414,18 +7448,18 @@
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B5" s="31"/>
+        <v>193</v>
+      </c>
+      <c r="B5" s="28"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="20">
+      <c r="D5" s="19">
         <v>0.01</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="19">
         <v>0</v>
       </c>
-      <c r="F5" s="24" t="s">
-        <v>170</v>
+      <c r="F5" s="23" t="s">
+        <v>169</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -7435,18 +7469,18 @@
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="20">
+      <c r="D6" s="19">
         <v>1</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="19">
         <v>0</v>
       </c>
-      <c r="F6" s="24" t="s">
-        <v>172</v>
+      <c r="F6" s="23" t="s">
+        <v>171</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -7458,8 +7492,8 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="24"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -7470,7 +7504,7 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="E8" s="20"/>
+      <c r="E8" s="19"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -7481,8 +7515,8 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -7493,9 +7527,9 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="24"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -7506,9 +7540,9 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="24"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -7559,6 +7593,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7754,6 +7789,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7795,42 +7831,42 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="M2" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="30" t="s">
         <v>108</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="27" t="s">
+      <c r="Q2" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="R2" s="28" t="s">
+      <c r="R2" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="S2" s="27" t="s">
+      <c r="S2" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="T2" s="28" t="s">
+      <c r="T2" s="30" t="s">
         <v>110</v>
       </c>
       <c r="U2" s="5"/>
@@ -8249,7 +8285,10 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8279,7 +8318,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -8530,6 +8569,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8678,6 +8718,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8710,10 +8751,10 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="30" t="s">
         <v>121</v>
       </c>
       <c r="I2" s="5"/>
@@ -8982,6 +9023,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9338,6 +9380,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9595,6 +9638,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9938,7 +9982,10 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="B2" sqref="B2:B6"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9968,7 +10015,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -10000,7 +10047,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -10032,7 +10079,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -10089,7 +10136,10 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10250,11 +10300,16 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3:C3"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="15.6640625" customWidth="1"/>
+    <col min="1" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="15.6640625" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10298,13 +10353,13 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="3"/>
@@ -10312,8 +10367,15 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>176</v>
+      </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -10403,11 +10465,11 @@
   </sheetData>
   <autoFilter ref="A2:H2"/>
   <dataValidations count="8">
-    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A3:A12">
+    <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Value must be a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_ ..." promptTitle="Id" prompt="Enter a unique string identifier that (a) is composed of letters, numbers and underscores; (b) is 63 characters or less; and (c) is not a decimal, hexadecimal, or scientific number_x000a__x000a_Enter a string._x000a__x000a_Value must be between 1 and 63 characters._x000a__x000a_Value mu ..." sqref="A5:A12">
       <formula1>1</formula1>
       <formula2>63</formula2>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B3:B12">
+    <dataValidation type="textLength" errorStyle="warning" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Value must be a string._x000a__x000a_Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Enter a string._x000a__x000a_Value must be less than or equal to 255 characters." sqref="B5:B12">
       <formula1>255</formula1>
     </dataValidation>
     <dataValidation errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Evidence" error="Value must be a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" promptTitle="Evidence" prompt="Enter a list of observations from &quot;Observations:A&quot;._x000a__x000a_Examples:_x000a_* Obs1(+, s=50, q=100); Obs2(-)_x000a_* Obs3(~, s=90)_x000a_* Obs4(+, q=30)" sqref="E3:E12"/>
@@ -10417,7 +10479,7 @@
     </dataValidation>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="H3:H12"/>
     <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" promptTitle="Identifiers" prompt="Enter a comma-separated list of identifiers in external namespaces._x000a__x000a_Examples:_x000a_* doi: 10.1016/j.tcb.2015.09.004_x000a_* chebi: CHEBI:15377, kegg.compound: C00001" sqref="D4:D12"/>
-    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Framework" error="Value must be a comma-separated list of WC ontology terms &quot;deterministic_simulation_algorithm&quot;, &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." promptTitle="Framework" prompt="Enter a comma-separated list of WC ontology terms &quot;deterministic_simulation_algorithm&quot;, &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." sqref="C5:C12 C3">
+    <dataValidation type="list" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Framework" error="Value must be a comma-separated list of WC ontology terms &quot;deterministic_simulation_algorithm&quot;, &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." promptTitle="Framework" prompt="Enter a comma-separated list of WC ontology terms &quot;deterministic_simulation_algorithm&quot;, &quot;dynamic_flux_balance_analysis&quot;, &quot;ordinary_differential_equations&quot;, &quot;stochastic_simulation_algorithm&quot;." sqref="C5:C12">
       <formula1>"deterministic_simulation_algorithm,dynamic_flux_balance_analysis,ordinary_differential_equations,stochastic_simulation_algorithm"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10434,11 +10496,17 @@
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="21" width="15.6640625" customWidth="1"/>
+    <col min="1" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="21" width="15.6640625" customWidth="1"/>
     <col min="22" max="22" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10475,29 +10543,29 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="30" t="s">
         <v>56</v>
       </c>
       <c r="L2" s="5"/>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="O2" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="28" t="s">
+      <c r="P2" s="30" t="s">
         <v>57</v>
       </c>
       <c r="Q2" s="5"/>
@@ -10582,15 +10650,15 @@
         <v>157</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>158</v>
+        <v>200</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="I4" s="9">
         <v>1</v>
@@ -10599,10 +10667,10 @@
         <v>0</v>
       </c>
       <c r="K4" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="L4" s="11" t="s">
         <v>161</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>162</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -10612,7 +10680,7 @@
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="U4" s="3"/>
     </row>
@@ -10837,7 +10905,7 @@
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Biological type" error="Value must be a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." promptTitle="Biological type" prompt="Enter a comma-separated list of WC ontology terms &quot;cellular_compartment&quot;, &quot;extracellular_compartment&quot; or blank." sqref="C4:C13">
       <formula1>"cellular_compartment,extracellular_compartment"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Physical type" error="Value must be a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." promptTitle="Physical type" prompt="Enter a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." sqref="D4:D13">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Physical type" error="Value must be a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." promptTitle="Physical type" prompt="Enter a comma-separated list of WC ontology terms &quot;fluid_compartment&quot;, &quot;membrane_compartment&quot; or blank." sqref="D5:D13">
       <formula1>"fluid_compartment,membrane_compartment"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Geometry" error="Value must be a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." promptTitle="Geometry" prompt="Enter a comma-separated list of WC ontology terms &quot;3D_compartment&quot; or blank." sqref="E4:E13">
@@ -10905,11 +10973,16 @@
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4:A5"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="14" width="15.6640625" customWidth="1"/>
+    <col min="1" max="12" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" customWidth="1"/>
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10934,22 +11007,22 @@
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="30" t="s">
         <v>69</v>
       </c>
       <c r="I2" s="5"/>
@@ -11005,10 +11078,10 @@
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -11021,22 +11094,22 @@
         <v>0</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -11049,13 +11122,13 @@
         <v>0</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N5" s="3"/>
     </row>
@@ -11239,7 +11312,10 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E3" sqref="E3:E4"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11295,17 +11371,17 @@
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>155</v>
       </c>
       <c r="E3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -11315,17 +11391,17 @@
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>155</v>
       </c>
       <c r="E4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -11484,7 +11560,10 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="1">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11548,23 +11627,23 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E3" s="17">
+        <v>159</v>
+      </c>
+      <c r="E3" s="16">
         <v>100</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -11574,23 +11653,23 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E4" s="15">
         <v>0</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="3">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -11632,7 +11711,6 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -11723,9 +11801,6 @@
     <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Mean" error="Value must be a float or blank." promptTitle="Mean" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="E3:E12">
       <formula1>-1E-100</formula1>
     </dataValidation>
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="F3:F12">
-      <formula1>-1E-100</formula1>
-    </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;molecule&quot;, &quot;molar&quot;, &quot;millimolar&quot;, &quot;micromolar&quot;, &quot;nanomolar&quot;, &quot;picomolar&quot;, &quot;femtomolar&quot;, &quot;attomolar&quot; or blank." sqref="G5:G12">
       <formula1>"molecule,molar,millimolar,micromolar,nanomolar,picomolar,femtomolar,attomolar"</formula1>
     </dataValidation>
@@ -11742,6 +11817,9 @@
     </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Units" error="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Value must be one unit of &quot;molecule&quot; or blank." promptTitle="Units" prompt="Units (e.g. 'second', 'meter', or 'gram')_x000a__x000a_Select one unit of &quot;molecule&quot; or blank." sqref="G3:G4">
       <formula1>"molecule"</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Standard deviation" error="Value must be a float or blank." promptTitle="Standard deviation" prompt="Enter a float or blank._x000a__x000a_Value must be greater than or equal to 0.0." sqref="F8:F12 F3:F6">
+      <formula1>-1E-100</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>